<commit_message>
end of day data collection
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester8.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3251467A-FB93-49A4-B616-7B47878D46B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A567DD90-C522-401F-8F6B-342F0DAC7B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1027,10 +1027,10 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>38.5</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.5</c:v>
@@ -1313,7 +1313,7 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0</c:v>
@@ -2053,7 +2053,7 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0</c:v>
@@ -3341,7 +3341,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>38.5</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3467,7 +3467,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>19</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4309,7 +4309,7 @@
                   <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3</c:v>
+                  <c:v>3.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4422,7 +4422,7 @@
                   <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.5</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8137,7 +8137,7 @@
   <dimension ref="A1:AG122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8204,11 +8204,11 @@
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>38.5</v>
+        <v>39</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F2" s="9">
         <f>SUM(F4:F150)</f>
@@ -8220,7 +8220,7 @@
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>122.5</v>
+        <v>124</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -8699,10 +8699,10 @@
         <v>0.5</v>
       </c>
       <c r="D18" s="15">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="E18" s="15">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="F18" s="15">
         <v>0</v>
@@ -8712,7 +8712,7 @@
       </c>
       <c r="H18" s="1">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10.5</v>
       </c>
       <c r="I18" s="24">
         <v>15</v>
@@ -8863,7 +8863,7 @@
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="14">
         <f>SUM(H18:H24)</f>
-        <v>9</v>
+        <v>10.5</v>
       </c>
       <c r="B26" s="17"/>
       <c r="C26" s="17"/>

</xml_diff>

<commit_message>
Lecture hall ranking updated
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester8.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97FCEA12-062B-4EC7-A471-7C7DB2F87E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE1B132-C7FC-4C9C-810A-0A40865CEFAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1021,22 +1021,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>39</c:v>
+                  <c:v>39.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>14.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>69</c:v>
+                  <c:v>69.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>38</c:v>
+                  <c:v>41.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>49</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1340,7 +1340,7 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>0</c:v>
@@ -2080,7 +2080,7 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>0</c:v>
@@ -3089,7 +3089,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>39</c:v>
+                  <c:v>39.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3341,7 +3341,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>69</c:v>
+                  <c:v>69.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3467,7 +3467,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>38</c:v>
+                  <c:v>41.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3719,7 +3719,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>49</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4109,6 +4109,9 @@
                 <c:pt idx="22">
                   <c:v>4</c:v>
                 </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4246,6 +4249,9 @@
                 <c:pt idx="22">
                   <c:v>0.5</c:v>
                 </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4383,6 +4389,9 @@
                 <c:pt idx="22">
                   <c:v>2</c:v>
                 </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4520,6 +4529,9 @@
                 <c:pt idx="22">
                   <c:v>2</c:v>
                 </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4657,6 +4669,9 @@
                 <c:pt idx="22">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4793,6 +4808,9 @@
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8281,7 +8299,7 @@
   <dimension ref="A1:AG122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8340,7 +8358,7 @@
       </c>
       <c r="B2" s="5">
         <f>SUM(B4:B166)</f>
-        <v>39</v>
+        <v>39.5</v>
       </c>
       <c r="C2" s="6">
         <f>SUM(C4:C150)</f>
@@ -8348,11 +8366,11 @@
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>69</v>
+        <v>69.5</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
-        <v>38</v>
+        <v>41.5</v>
       </c>
       <c r="F2" s="9">
         <f>SUM(F4:F150)</f>
@@ -8360,11 +8378,11 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(G4:G150)</f>
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>210</v>
+        <v>216.5</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -8448,8 +8466,8 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" s="21">
-        <f>AVERAGE(H4:H25)</f>
-        <v>9.045454545454545</v>
+        <f>AVERAGE(H4:H26)</f>
+        <v>9.1304347826086953</v>
       </c>
       <c r="B6" s="15">
         <v>0</v>
@@ -9123,15 +9141,27 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
+      <c r="B27" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="C27" s="17">
+        <v>0</v>
+      </c>
+      <c r="D27" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="E27" s="17">
+        <v>3.5</v>
+      </c>
+      <c r="F27" s="17">
+        <v>0</v>
+      </c>
+      <c r="G27" s="17">
+        <v>2</v>
+      </c>
       <c r="H27" s="1">
         <f>SUM(B27:G27)</f>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="I27" s="24">
         <v>24</v>
@@ -9242,7 +9272,7 @@
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="19">
         <f>SUM(H25:H31)</f>
-        <v>22</v>
+        <v>28.5</v>
       </c>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>

</xml_diff>

<commit_message>
Panix @ the Disco
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester8.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D242A5AC-67BB-4A18-A3D5-C557A57CBB4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E26ACFED-46B5-494C-B578-6F0FE8169C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1027,10 +1027,10 @@
                   <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>85.5</c:v>
+                  <c:v>86.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>50</c:v>
+                  <c:v>52.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.5</c:v>
@@ -1355,7 +1355,7 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>7.5</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>0</c:v>
@@ -2095,7 +2095,7 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>7.5</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>0</c:v>
@@ -3341,7 +3341,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>85.5</c:v>
+                  <c:v>86.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3467,7 +3467,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>50</c:v>
+                  <c:v>52.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4435,7 +4435,7 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4590,7 +4590,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>3.5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8389,7 +8389,7 @@
   <dimension ref="A1:AG122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8456,11 +8456,11 @@
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>85.5</v>
+        <v>86.5</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
-        <v>50</v>
+        <v>52.5</v>
       </c>
       <c r="F2" s="9">
         <f>SUM(F4:F150)</f>
@@ -8472,7 +8472,7 @@
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>267</v>
+        <v>270.5</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -9397,10 +9397,10 @@
         <v>0</v>
       </c>
       <c r="D32" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E32" s="15">
-        <v>3.5</v>
+        <v>6</v>
       </c>
       <c r="F32" s="15">
         <v>0</v>
@@ -9410,7 +9410,7 @@
       </c>
       <c r="H32" s="1">
         <f t="shared" si="1"/>
-        <v>7.5</v>
+        <v>11</v>
       </c>
       <c r="I32" s="24">
         <v>29</v>
@@ -9561,7 +9561,7 @@
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="14">
         <f>SUM(H32:H38)</f>
-        <v>7.5</v>
+        <v>11</v>
       </c>
       <c r="B40" s="17"/>
       <c r="C40" s="17"/>

</xml_diff>

<commit_message>
sesh and work update
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester8.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AABEB4FA-B28E-4557-BC10-75817AF9F75E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF5BC5F-6D1E-495E-BCC9-C053842F2E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1021,22 +1021,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>52</c:v>
+                  <c:v>55.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23</c:v>
+                  <c:v>23.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>99.5</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>61.5</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>74</c:v>
+                  <c:v>75.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1364,10 +1364,10 @@
                   <c:v>14.5</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>7</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>0</c:v>
@@ -2104,10 +2104,10 @@
                   <c:v>14.5</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>7</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>0</c:v>
@@ -3089,7 +3089,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>52</c:v>
+                  <c:v>55.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3215,7 +3215,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>23</c:v>
+                  <c:v>23.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3341,7 +3341,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>99.5</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3467,7 +3467,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>61.5</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3719,7 +3719,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>74</c:v>
+                  <c:v>75.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4133,6 +4133,12 @@
                 <c:pt idx="30">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="31">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4294,6 +4300,9 @@
                 <c:pt idx="30">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4456,7 +4465,10 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3</c:v>
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4619,6 +4631,12 @@
                 <c:pt idx="30">
                   <c:v>3.5</c:v>
                 </c:pt>
+                <c:pt idx="31">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4783,6 +4801,9 @@
                 <c:pt idx="31">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4946,6 +4967,9 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8433,8 +8457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE33D67F-891D-4EAD-9F40-3D033E7F434D}">
   <dimension ref="A1:AG122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8493,19 +8517,19 @@
       </c>
       <c r="B2" s="5">
         <f>SUM(B4:B166)</f>
-        <v>52</v>
+        <v>55.5</v>
       </c>
       <c r="C2" s="6">
         <f>SUM(C4:C150)</f>
-        <v>23</v>
+        <v>23.5</v>
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>99.5</v>
+        <v>104</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
-        <v>61.5</v>
+        <v>63</v>
       </c>
       <c r="F2" s="9">
         <f>SUM(F4:F150)</f>
@@ -8513,11 +8537,11 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(G4:G150)</f>
-        <v>74</v>
+        <v>75.5</v>
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>310.5</v>
+        <v>322</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -8601,8 +8625,8 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" s="21">
-        <f>AVERAGE(H4:H34)</f>
-        <v>9.7903225806451619</v>
+        <f>AVERAGE(H4:H35)</f>
+        <v>9.859375</v>
       </c>
       <c r="B6" s="15">
         <v>0</v>
@@ -9529,12 +9553,18 @@
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
+      <c r="B35" s="15">
+        <v>1</v>
+      </c>
+      <c r="C35" s="15">
+        <v>0.5</v>
+      </c>
       <c r="D35" s="15">
-        <v>3</v>
-      </c>
-      <c r="E35" s="15"/>
+        <v>5.5</v>
+      </c>
+      <c r="E35" s="15">
+        <v>1</v>
+      </c>
       <c r="F35" s="15">
         <v>0</v>
       </c>
@@ -9543,7 +9573,7 @@
       </c>
       <c r="H35" s="1">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="I35" s="24">
         <v>32</v>
@@ -9556,15 +9586,25 @@
       <c r="A36" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="15"/>
+      <c r="B36" s="15">
+        <v>2.5</v>
+      </c>
       <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="15"/>
+      <c r="D36" s="15">
+        <v>2</v>
+      </c>
+      <c r="E36" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="F36" s="15">
+        <v>0</v>
+      </c>
+      <c r="G36" s="15">
+        <v>1.5</v>
+      </c>
       <c r="H36" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="I36" s="24">
         <v>33</v>
@@ -9636,7 +9676,7 @@
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="14">
         <f>SUM(H32:H38)</f>
-        <v>51</v>
+        <v>62.5</v>
       </c>
       <c r="B40" s="17"/>
       <c r="C40" s="17"/>

</xml_diff>

<commit_message>
One out of three, still going
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester8.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6AAB85-DBA1-4993-8D29-097BFE45F4C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D33A0A4C-0C2A-4821-AC8E-F5C34E5FEF42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1021,22 +1021,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>68.5</c:v>
+                  <c:v>72.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27.5</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>128.5</c:v>
+                  <c:v>142.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>72.5</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>91</c:v>
+                  <c:v>91.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1385,10 +1385,10 @@
                   <c:v>14.5</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>7</c:v>
+                  <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>0</c:v>
@@ -2125,10 +2125,10 @@
                   <c:v>14.5</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>7</c:v>
+                  <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>0</c:v>
@@ -3089,7 +3089,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>68.5</c:v>
+                  <c:v>72.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3215,7 +3215,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>27.5</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3341,7 +3341,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>128.5</c:v>
+                  <c:v>142.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3467,7 +3467,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>72.5</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3719,7 +3719,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>91</c:v>
+                  <c:v>91.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4155,7 +4155,10 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1</c:v>
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4342,6 +4345,9 @@
                 <c:pt idx="38">
                   <c:v>0.5</c:v>
                 </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4525,7 +4531,10 @@
                   <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1.5</c:v>
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>12.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4709,6 +4718,12 @@
                 <c:pt idx="37">
                   <c:v>3</c:v>
                 </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4894,6 +4909,9 @@
                 <c:pt idx="38">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="39">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5078,6 +5096,9 @@
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8566,7 +8587,7 @@
   <dimension ref="A1:AG122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8625,19 +8646,19 @@
       </c>
       <c r="B2" s="5">
         <f>SUM(B4:B166)</f>
-        <v>68.5</v>
+        <v>72.5</v>
       </c>
       <c r="C2" s="6">
         <f>SUM(C4:C150)</f>
-        <v>27.5</v>
+        <v>28</v>
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>128.5</v>
+        <v>142.5</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
-        <v>72.5</v>
+        <v>75</v>
       </c>
       <c r="F2" s="9">
         <f>SUM(F4:F150)</f>
@@ -8645,11 +8666,11 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(G4:G150)</f>
-        <v>91</v>
+        <v>91.5</v>
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>388.5</v>
+        <v>410</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -8733,8 +8754,8 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" s="21">
-        <f>AVERAGE(H4:H41)</f>
-        <v>10.039473684210526</v>
+        <f>AVERAGE(H4:H43)</f>
+        <v>10.25</v>
       </c>
       <c r="B6" s="15">
         <v>0</v>
@@ -9885,15 +9906,17 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B42" s="17">
-        <v>1</v>
+        <v>4.5</v>
       </c>
       <c r="C42" s="17">
         <v>0.5</v>
       </c>
       <c r="D42" s="17">
+        <v>3</v>
+      </c>
+      <c r="E42" s="17">
         <v>1.5</v>
       </c>
-      <c r="E42" s="17"/>
       <c r="F42" s="17">
         <v>0</v>
       </c>
@@ -9902,7 +9925,7 @@
       </c>
       <c r="H42" s="1">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>13.5</v>
       </c>
       <c r="I42" s="24">
         <v>39</v>
@@ -9915,15 +9938,27 @@
       <c r="A43" t="s">
         <v>34</v>
       </c>
-      <c r="B43" s="17"/>
-      <c r="C43" s="17"/>
-      <c r="D43" s="17"/>
-      <c r="E43" s="17"/>
-      <c r="F43" s="17"/>
-      <c r="G43" s="17"/>
+      <c r="B43" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="C43" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="D43" s="17">
+        <v>12.5</v>
+      </c>
+      <c r="E43" s="17">
+        <v>1</v>
+      </c>
+      <c r="F43" s="17">
+        <v>0</v>
+      </c>
+      <c r="G43" s="17">
+        <v>0.5</v>
+      </c>
       <c r="H43" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="I43" s="24">
         <v>40</v>
@@ -9995,7 +10030,7 @@
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="19">
         <f>SUM(H39:H45)</f>
-        <v>50</v>
+        <v>71.5</v>
       </c>
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>

</xml_diff>

<commit_message>
Less than I should, more than you'd think
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester8.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D33A0A4C-0C2A-4821-AC8E-F5C34E5FEF42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19306B29-C212-46EE-9DC2-DD360AB04D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1021,22 +1021,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>72.5</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28</c:v>
+                  <c:v>28.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>142.5</c:v>
+                  <c:v>154</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>75</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>91.5</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1391,7 +1391,7 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>0</c:v>
@@ -2131,7 +2131,7 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>0</c:v>
@@ -3089,7 +3089,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>72.5</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3215,7 +3215,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>28</c:v>
+                  <c:v>28.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3341,7 +3341,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>142.5</c:v>
+                  <c:v>154</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3467,7 +3467,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>75</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3719,7 +3719,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>91.5</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4160,6 +4160,9 @@
                 <c:pt idx="39">
                   <c:v>0.5</c:v>
                 </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4348,6 +4351,9 @@
                 <c:pt idx="39">
                   <c:v>0.5</c:v>
                 </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4536,6 +4542,9 @@
                 <c:pt idx="39">
                   <c:v>12.5</c:v>
                 </c:pt>
+                <c:pt idx="40">
+                  <c:v>11.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4724,6 +4733,9 @@
                 <c:pt idx="39">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="40">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4912,6 +4924,9 @@
                 <c:pt idx="39">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="40">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5098,6 +5113,9 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="39">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="40">
                   <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
@@ -8586,8 +8604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE33D67F-891D-4EAD-9F40-3D033E7F434D}">
   <dimension ref="A1:AG122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8646,19 +8664,19 @@
       </c>
       <c r="B2" s="5">
         <f>SUM(B4:B166)</f>
-        <v>72.5</v>
+        <v>73</v>
       </c>
       <c r="C2" s="6">
         <f>SUM(C4:C150)</f>
-        <v>28</v>
+        <v>28.5</v>
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>142.5</v>
+        <v>154</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F2" s="9">
         <f>SUM(F4:F150)</f>
@@ -8666,11 +8684,11 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(G4:G150)</f>
-        <v>91.5</v>
+        <v>92</v>
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>410</v>
+        <v>424</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -9968,15 +9986,27 @@
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B44" s="17"/>
-      <c r="C44" s="17"/>
-      <c r="D44" s="17"/>
-      <c r="E44" s="17"/>
-      <c r="F44" s="17"/>
-      <c r="G44" s="17"/>
+      <c r="B44" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="C44" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="D44" s="17">
+        <v>11.5</v>
+      </c>
+      <c r="E44" s="17">
+        <v>1</v>
+      </c>
+      <c r="F44" s="17">
+        <v>0</v>
+      </c>
+      <c r="G44" s="17">
+        <v>0.5</v>
+      </c>
       <c r="H44" s="1">
         <f>SUM(B44:G44)</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="I44" s="24">
         <v>41</v>
@@ -10030,7 +10060,7 @@
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="19">
         <f>SUM(H39:H45)</f>
-        <v>71.5</v>
+        <v>85.5</v>
       </c>
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>

</xml_diff>

<commit_message>
End of feb com
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester8.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D73DE52F-13FB-45C2-8749-B191F0616A27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480773ED-23B2-4801-82BB-356356AEB7A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1021,22 +1021,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>73.25</c:v>
+                  <c:v>73.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>28.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>163</c:v>
+                  <c:v>172</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>77</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>92</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1397,7 +1397,7 @@
                   <c:v>10.25</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0</c:v>
+                  <c:v>12.25</c:v>
                 </c:pt>
                 <c:pt idx="43">
                   <c:v>0</c:v>
@@ -2137,7 +2137,7 @@
                   <c:v>10.25</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0</c:v>
+                  <c:v>12.25</c:v>
                 </c:pt>
                 <c:pt idx="43">
                   <c:v>0</c:v>
@@ -3089,7 +3089,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>73.25</c:v>
+                  <c:v>73.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3341,7 +3341,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>163</c:v>
+                  <c:v>172</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3467,7 +3467,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>77</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3719,7 +3719,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>92</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4166,6 +4166,9 @@
                 <c:pt idx="41">
                   <c:v>0.25</c:v>
                 </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4554,6 +4557,9 @@
                 <c:pt idx="41">
                   <c:v>9</c:v>
                 </c:pt>
+                <c:pt idx="42">
+                  <c:v>9</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4748,6 +4754,9 @@
                 <c:pt idx="41">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="42">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5135,6 +5144,9 @@
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8623,7 +8635,7 @@
   <dimension ref="A1:AG122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8682,7 +8694,7 @@
       </c>
       <c r="B2" s="5">
         <f>SUM(B4:B166)</f>
-        <v>73.25</v>
+        <v>73.5</v>
       </c>
       <c r="C2" s="6">
         <f>SUM(C4:C150)</f>
@@ -8690,11 +8702,11 @@
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F2" s="9">
         <f>SUM(F4:F150)</f>
@@ -8702,11 +8714,11 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(G4:G150)</f>
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>434.25</v>
+        <v>446.5</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -10070,15 +10082,23 @@
       <c r="A46" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B46" s="15"/>
+      <c r="B46" s="15">
+        <v>0.25</v>
+      </c>
       <c r="C46" s="15"/>
-      <c r="D46" s="15"/>
-      <c r="E46" s="15"/>
+      <c r="D46" s="15">
+        <v>9</v>
+      </c>
+      <c r="E46" s="15">
+        <v>1</v>
+      </c>
       <c r="F46" s="15"/>
-      <c r="G46" s="15"/>
+      <c r="G46" s="15">
+        <v>2</v>
+      </c>
       <c r="H46" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>12.25</v>
       </c>
       <c r="I46" s="24">
         <v>43</v>
@@ -10229,7 +10249,7 @@
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="14">
         <f>SUM(H46:H52)</f>
-        <v>0</v>
+        <v>12.25</v>
       </c>
       <c r="B54" s="17"/>
       <c r="C54" s="17"/>

</xml_diff>

<commit_message>
Something's got to giver
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester8.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F9B7B3-CCA7-4F8E-899A-A60D65D9A6A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F29F7BED-C8C8-4A9B-B0CC-8DCF28E688AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1027,16 +1027,16 @@
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>183.5</c:v>
+                  <c:v>193</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>80.5</c:v>
+                  <c:v>83.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>94.5</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1403,7 +1403,7 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>0</c:v>
@@ -2143,7 +2143,7 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>0</c:v>
@@ -3341,7 +3341,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>183.5</c:v>
+                  <c:v>193</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3467,7 +3467,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>80.5</c:v>
+                  <c:v>83.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3719,7 +3719,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>94.5</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4172,6 +4172,9 @@
                 <c:pt idx="43">
                   <c:v>0.5</c:v>
                 </c:pt>
+                <c:pt idx="44">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4372,6 +4375,9 @@
                 <c:pt idx="43">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="44">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4572,6 +4578,9 @@
                 <c:pt idx="43">
                   <c:v>10.5</c:v>
                 </c:pt>
+                <c:pt idx="44">
+                  <c:v>9.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4772,6 +4781,9 @@
                 <c:pt idx="43">
                   <c:v>2.5</c:v>
                 </c:pt>
+                <c:pt idx="44">
+                  <c:v>3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4972,6 +4984,9 @@
                 <c:pt idx="43">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="44">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5171,6 +5186,9 @@
                 </c:pt>
                 <c:pt idx="43">
                   <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8658,8 +8676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE33D67F-891D-4EAD-9F40-3D033E7F434D}">
   <dimension ref="A1:AG122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8726,11 +8744,11 @@
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>183.5</v>
+        <v>193</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
-        <v>80.5</v>
+        <v>83.5</v>
       </c>
       <c r="F2" s="9">
         <f>SUM(F4:F150)</f>
@@ -8738,11 +8756,11 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(G4:G150)</f>
-        <v>94.5</v>
+        <v>97</v>
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>463</v>
+        <v>478</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -10170,15 +10188,27 @@
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B48" s="15"/>
-      <c r="C48" s="15"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="15"/>
-      <c r="F48" s="15"/>
-      <c r="G48" s="15"/>
+      <c r="B48" s="15">
+        <v>0</v>
+      </c>
+      <c r="C48" s="15">
+        <v>0</v>
+      </c>
+      <c r="D48" s="15">
+        <v>9.5</v>
+      </c>
+      <c r="E48" s="15">
+        <v>3</v>
+      </c>
+      <c r="F48" s="15">
+        <v>0</v>
+      </c>
+      <c r="G48" s="15">
+        <v>2.5</v>
+      </c>
       <c r="H48" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="I48" s="24">
         <v>45</v>
@@ -10289,7 +10319,7 @@
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="14">
         <f>SUM(H46:H52)</f>
-        <v>28.75</v>
+        <v>43.75</v>
       </c>
       <c r="B54" s="17"/>
       <c r="C54" s="17"/>

</xml_diff>

<commit_message>
Might be all I have
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester8.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD8FBE8-58E9-408A-93AA-B6419DEC0FA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B98AC0BD-34BE-4F9B-9328-B3184DE26B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1021,13 +1021,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>86.5</c:v>
+                  <c:v>89.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>213.5</c:v>
+                  <c:v>214</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>98.5</c:v>
@@ -1036,7 +1036,7 @@
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>115</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1427,7 +1427,7 @@
                   <c:v>14.5</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="53">
                   <c:v>0</c:v>
@@ -2167,7 +2167,7 @@
                   <c:v>14.5</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="53">
                   <c:v>0</c:v>
@@ -3089,7 +3089,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>86.5</c:v>
+                  <c:v>89.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3215,7 +3215,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>43</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3341,7 +3341,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>213.5</c:v>
+                  <c:v>214</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3719,7 +3719,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>115</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4196,6 +4196,9 @@
                 <c:pt idx="51">
                   <c:v>4</c:v>
                 </c:pt>
+                <c:pt idx="52">
+                  <c:v>3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4420,6 +4423,9 @@
                 <c:pt idx="51">
                   <c:v>3.5</c:v>
                 </c:pt>
+                <c:pt idx="52">
+                  <c:v>2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4644,6 +4650,9 @@
                 <c:pt idx="51">
                   <c:v>1.5</c:v>
                 </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5092,6 +5101,9 @@
                 <c:pt idx="51">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="52">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5315,6 +5327,9 @@
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8802,8 +8817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE33D67F-891D-4EAD-9F40-3D033E7F434D}">
   <dimension ref="A1:AG122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8862,15 +8877,15 @@
       </c>
       <c r="B2" s="5">
         <f>SUM(B4:B166)</f>
-        <v>86.5</v>
+        <v>89.5</v>
       </c>
       <c r="C2" s="6">
         <f>SUM(C4:C150)</f>
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>213.5</v>
+        <v>214</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
@@ -8882,11 +8897,11 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(G4:G150)</f>
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>557</v>
+        <v>566.5</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -8970,8 +8985,8 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" s="21">
-        <f>AVERAGE(H4:H53)</f>
-        <v>10.61</v>
+        <f>AVERAGE(H4:H56)</f>
+        <v>10.688679245283019</v>
       </c>
       <c r="B6" s="15">
         <v>0</v>
@@ -10567,15 +10582,25 @@
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B56" s="17"/>
-      <c r="C56" s="17"/>
-      <c r="D56" s="17"/>
+      <c r="B56" s="17">
+        <v>3</v>
+      </c>
+      <c r="C56" s="17">
+        <v>2</v>
+      </c>
+      <c r="D56" s="17">
+        <v>0.5</v>
+      </c>
       <c r="E56" s="17"/>
-      <c r="F56" s="17"/>
-      <c r="G56" s="17"/>
+      <c r="F56" s="17">
+        <v>0</v>
+      </c>
+      <c r="G56" s="17">
+        <v>4</v>
+      </c>
       <c r="H56" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>9.5</v>
       </c>
       <c r="I56" s="24">
         <v>53</v>
@@ -10668,7 +10693,7 @@
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="19">
         <f>SUM(H53:H59)</f>
-        <v>38.5</v>
+        <v>48</v>
       </c>
       <c r="B61" s="15"/>
       <c r="C61" s="15"/>

</xml_diff>

<commit_message>
updated work and ses data
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester8.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3500AE4-64B8-4308-B278-680EDFE11003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370795DD-1995-44AB-BBC4-F2A0C63A8602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1021,22 +1021,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>97</c:v>
+                  <c:v>98.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>49</c:v>
+                  <c:v>51.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>232</c:v>
+                  <c:v>235</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>109.5</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>150</c:v>
+                  <c:v>157</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1460,10 +1460,10 @@
                   <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0</c:v>
+                  <c:v>14.5</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>0</c:v>
@@ -2200,10 +2200,10 @@
                   <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0</c:v>
+                  <c:v>14.5</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>0</c:v>
@@ -3089,7 +3089,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>97</c:v>
+                  <c:v>98.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3215,7 +3215,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>49</c:v>
+                  <c:v>51.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3341,7 +3341,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>232</c:v>
+                  <c:v>235</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3467,7 +3467,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>109.5</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3593,7 +3593,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3719,7 +3719,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>150</c:v>
+                  <c:v>157</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4229,6 +4229,12 @@
                 <c:pt idx="62">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4486,6 +4492,12 @@
                 <c:pt idx="62">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4743,6 +4755,12 @@
                 <c:pt idx="62">
                   <c:v>3</c:v>
                 </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5000,6 +5018,12 @@
                 <c:pt idx="62">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="63">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5257,6 +5281,12 @@
                 <c:pt idx="62">
                   <c:v>0.5</c:v>
                 </c:pt>
+                <c:pt idx="63">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5513,6 +5543,12 @@
                 </c:pt>
                 <c:pt idx="62">
                   <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>4.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9000,8 +9036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE33D67F-891D-4EAD-9F40-3D033E7F434D}">
   <dimension ref="A1:AG122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9060,31 +9096,31 @@
       </c>
       <c r="B2" s="5">
         <f>SUM(B4:B166)</f>
-        <v>97</v>
+        <v>98.5</v>
       </c>
       <c r="C2" s="6">
         <f>SUM(C4:C150)</f>
-        <v>49</v>
+        <v>51.5</v>
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
-        <v>109.5</v>
+        <v>119</v>
       </c>
       <c r="F2" s="9">
         <f>SUM(F4:F150)</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="G2" s="4">
         <f>SUM(G4:G150)</f>
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>638.5</v>
+        <v>663.5</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -11117,15 +11153,27 @@
       <c r="A67" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B67" s="17"/>
-      <c r="C67" s="17"/>
-      <c r="D67" s="17"/>
-      <c r="E67" s="17"/>
-      <c r="F67" s="17"/>
-      <c r="G67" s="17"/>
+      <c r="B67" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="C67" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="D67" s="17">
+        <v>1.5</v>
+      </c>
+      <c r="E67" s="17">
+        <v>8.5</v>
+      </c>
+      <c r="F67" s="17">
+        <v>1</v>
+      </c>
+      <c r="G67" s="17">
+        <v>2.5</v>
+      </c>
       <c r="H67" s="1">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="I67" s="24">
         <v>64</v>
@@ -11139,15 +11187,27 @@
         <f>SUM(H60:H66)</f>
         <v>41.5</v>
       </c>
-      <c r="B68" s="17"/>
-      <c r="C68" s="17"/>
-      <c r="D68" s="17"/>
-      <c r="E68" s="17"/>
-      <c r="F68" s="17"/>
-      <c r="G68" s="17"/>
+      <c r="B68" s="17">
+        <v>1</v>
+      </c>
+      <c r="C68" s="17">
+        <v>2</v>
+      </c>
+      <c r="D68" s="17">
+        <v>1.5</v>
+      </c>
+      <c r="E68" s="17">
+        <v>1</v>
+      </c>
+      <c r="F68" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="G68" s="17">
+        <v>4.5</v>
+      </c>
       <c r="H68" s="1">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>10.5</v>
       </c>
       <c r="I68" s="24">
         <v>65</v>
@@ -11273,7 +11333,7 @@
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" s="19">
         <f>SUM(H67:H73)</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B75" s="15"/>
       <c r="C75" s="15"/>

</xml_diff>

<commit_message>
Try not to cry. cry
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester8.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370795DD-1995-44AB-BBC4-F2A0C63A8602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56ADC85C-F13B-4F37-B6D5-8F0CEE72C629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1021,22 +1021,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>98.5</c:v>
+                  <c:v>108</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>51.5</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>235</c:v>
+                  <c:v>235.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>119</c:v>
+                  <c:v>125.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>157</c:v>
+                  <c:v>159</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1463,10 +1463,10 @@
                   <c:v>14.5</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>10.5</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0</c:v>
+                  <c:v>14.5</c:v>
                 </c:pt>
                 <c:pt idx="66">
                   <c:v>0</c:v>
@@ -2203,10 +2203,10 @@
                   <c:v>14.5</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>10.5</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0</c:v>
+                  <c:v>14.5</c:v>
                 </c:pt>
                 <c:pt idx="66">
                   <c:v>0</c:v>
@@ -3089,7 +3089,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>98.5</c:v>
+                  <c:v>108</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3215,7 +3215,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>51.5</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3341,7 +3341,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>235</c:v>
+                  <c:v>235.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3467,7 +3467,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>119</c:v>
+                  <c:v>125.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3719,7 +3719,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>157</c:v>
+                  <c:v>159</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4233,7 +4233,10 @@
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>1</c:v>
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4498,6 +4501,9 @@
                 <c:pt idx="64">
                   <c:v>2</c:v>
                 </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4761,6 +4767,9 @@
                 <c:pt idx="64">
                   <c:v>1.5</c:v>
                 </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5022,7 +5031,10 @@
                   <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>3.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5287,6 +5299,9 @@
                 <c:pt idx="64">
                   <c:v>0.5</c:v>
                 </c:pt>
+                <c:pt idx="65">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5549,6 +5564,9 @@
                 </c:pt>
                 <c:pt idx="64">
                   <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9036,8 +9054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE33D67F-891D-4EAD-9F40-3D033E7F434D}">
   <dimension ref="A1:AG122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9096,19 +9114,19 @@
       </c>
       <c r="B2" s="5">
         <f>SUM(B4:B166)</f>
-        <v>98.5</v>
+        <v>108</v>
       </c>
       <c r="C2" s="6">
         <f>SUM(C4:C150)</f>
-        <v>51.5</v>
+        <v>52</v>
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>235</v>
+        <v>235.5</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
-        <v>119</v>
+        <v>125.5</v>
       </c>
       <c r="F2" s="9">
         <f>SUM(F4:F150)</f>
@@ -9116,11 +9134,11 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(G4:G150)</f>
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>663.5</v>
+        <v>682.5</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -11188,7 +11206,7 @@
         <v>41.5</v>
       </c>
       <c r="B68" s="17">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="C68" s="17">
         <v>2</v>
@@ -11197,7 +11215,7 @@
         <v>1.5</v>
       </c>
       <c r="E68" s="17">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F68" s="17">
         <v>0.5</v>
@@ -11207,7 +11225,7 @@
       </c>
       <c r="H68" s="1">
         <f t="shared" si="5"/>
-        <v>10.5</v>
+        <v>15</v>
       </c>
       <c r="I68" s="24">
         <v>65</v>
@@ -11217,15 +11235,27 @@
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B69" s="17"/>
-      <c r="C69" s="17"/>
-      <c r="D69" s="17"/>
-      <c r="E69" s="17"/>
-      <c r="F69" s="17"/>
-      <c r="G69" s="17"/>
+      <c r="B69" s="17">
+        <v>8</v>
+      </c>
+      <c r="C69" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="D69" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="E69" s="17">
+        <v>3.5</v>
+      </c>
+      <c r="F69" s="17">
+        <v>0</v>
+      </c>
+      <c r="G69" s="17">
+        <v>2</v>
+      </c>
       <c r="H69" s="1">
         <f t="shared" ref="H69:H74" si="6">SUM(B69:G69)</f>
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="I69" s="24">
         <v>66</v>
@@ -11333,7 +11363,7 @@
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" s="19">
         <f>SUM(H67:H73)</f>
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="B75" s="15"/>
       <c r="C75" s="15"/>

</xml_diff>

<commit_message>
Pride cometh before the fall
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester8.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56ADC85C-F13B-4F37-B6D5-8F0CEE72C629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31C5835-11BD-4382-94A3-1C5AA972B0EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1024,19 +1024,19 @@
                   <c:v>108</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>52</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>235.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>125.5</c:v>
+                  <c:v>126</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>159</c:v>
+                  <c:v>162.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1469,7 +1469,7 @@
                   <c:v>14.5</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="67">
                   <c:v>0</c:v>
@@ -2209,7 +2209,7 @@
                   <c:v>14.5</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="67">
                   <c:v>0</c:v>
@@ -3215,7 +3215,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>52</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3467,7 +3467,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>125.5</c:v>
+                  <c:v>126</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3719,7 +3719,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>159</c:v>
+                  <c:v>162.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4504,6 +4504,9 @@
                 <c:pt idx="65">
                   <c:v>0.5</c:v>
                 </c:pt>
+                <c:pt idx="66">
+                  <c:v>3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5036,6 +5039,9 @@
                 <c:pt idx="65">
                   <c:v>3.5</c:v>
                 </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5302,6 +5308,9 @@
                 <c:pt idx="65">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="66">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5567,6 +5576,9 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>3.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9054,8 +9066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE33D67F-891D-4EAD-9F40-3D033E7F434D}">
   <dimension ref="A1:AG122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9118,7 +9130,7 @@
       </c>
       <c r="C2" s="6">
         <f>SUM(C4:C150)</f>
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
@@ -9126,7 +9138,7 @@
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
-        <v>125.5</v>
+        <v>126</v>
       </c>
       <c r="F2" s="9">
         <f>SUM(F4:F150)</f>
@@ -9134,11 +9146,11 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(G4:G150)</f>
-        <v>159</v>
+        <v>162.5</v>
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>682.5</v>
+        <v>689.5</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -9222,8 +9234,8 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" s="21">
-        <f>AVERAGE(H4:H66)</f>
-        <v>10.134920634920634</v>
+        <f>AVERAGE(H4:H69)</f>
+        <v>10.340909090909092</v>
       </c>
       <c r="B6" s="15">
         <v>0</v>
@@ -11266,14 +11278,22 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B70" s="17"/>
-      <c r="C70" s="17"/>
+      <c r="C70" s="17">
+        <v>3</v>
+      </c>
       <c r="D70" s="17"/>
-      <c r="E70" s="17"/>
-      <c r="F70" s="17"/>
-      <c r="G70" s="17"/>
+      <c r="E70" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="F70" s="17">
+        <v>0</v>
+      </c>
+      <c r="G70" s="17">
+        <v>3.5</v>
+      </c>
       <c r="H70" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I70" s="24">
         <v>67</v>
@@ -11363,7 +11383,7 @@
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" s="19">
         <f>SUM(H67:H73)</f>
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B75" s="15"/>
       <c r="C75" s="15"/>

</xml_diff>

<commit_message>
slightly behind - update
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester8.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E4B9D3-22B2-4FAE-8A28-D1AAD0063EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44FF69A5-6224-4B39-AF38-09287B00E74D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1021,22 +1021,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>154.5</c:v>
+                  <c:v>157.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>87</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>316</c:v>
+                  <c:v>324</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>168</c:v>
+                  <c:v>171</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>193.5</c:v>
+                  <c:v>199.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1529,22 +1529,22 @@
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>9.5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>9.5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>2</c:v>
+                  <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="92">
                   <c:v>0</c:v>
@@ -2269,22 +2269,22 @@
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>9.5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>9.5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>2</c:v>
+                  <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="92">
                   <c:v>0</c:v>
@@ -3089,7 +3089,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>154.5</c:v>
+                  <c:v>157.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3215,7 +3215,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>87</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3341,7 +3341,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>316</c:v>
+                  <c:v>324</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3467,7 +3467,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>168</c:v>
+                  <c:v>171</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3719,7 +3719,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>193.5</c:v>
+                  <c:v>199.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4307,6 +4307,12 @@
                 <c:pt idx="88">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="89">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4639,6 +4645,15 @@
                 <c:pt idx="87">
                   <c:v>2</c:v>
                 </c:pt>
+                <c:pt idx="88">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4971,6 +4986,15 @@
                 <c:pt idx="87">
                   <c:v>4</c:v>
                 </c:pt>
+                <c:pt idx="88">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5306,6 +5330,12 @@
                 <c:pt idx="88">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="89">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>1.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5641,6 +5671,15 @@
                 <c:pt idx="88">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="89">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5968,13 +6007,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>2</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9462,8 +9510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE33D67F-891D-4EAD-9F40-3D033E7F434D}">
   <dimension ref="A1:AG122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D92" sqref="D92"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D95" sqref="D95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9522,19 +9570,19 @@
       </c>
       <c r="B2" s="5">
         <f>SUM(B4:B166)</f>
-        <v>154.5</v>
+        <v>157.5</v>
       </c>
       <c r="C2" s="6">
         <f>SUM(C4:C150)</f>
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>316</v>
+        <v>324</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="F2" s="9">
         <f>SUM(F4:F150)</f>
@@ -9542,11 +9590,11 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(G4:G150)</f>
-        <v>193.5</v>
+        <v>199.5</v>
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>921.5</v>
+        <v>942.5</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -9630,8 +9678,8 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" s="21">
-        <f>AVERAGE(H4:H88)</f>
-        <v>10.441176470588236</v>
+        <f>AVERAGE(H4:H94)</f>
+        <v>10.324175824175825</v>
       </c>
       <c r="B6" s="15">
         <v>0</v>
@@ -12325,11 +12373,11 @@
         <v>0</v>
       </c>
       <c r="G90" s="15">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="H90" s="1">
         <f t="shared" si="9"/>
-        <v>9.5</v>
+        <v>10</v>
       </c>
       <c r="I90" s="24">
         <v>87</v>
@@ -12355,11 +12403,11 @@
         <v>0</v>
       </c>
       <c r="G91" s="15">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H91" s="1">
         <f t="shared" si="9"/>
-        <v>9.5</v>
+        <v>10</v>
       </c>
       <c r="I91" s="24">
         <v>88</v>
@@ -12375,8 +12423,12 @@
       <c r="B92" s="15">
         <v>1</v>
       </c>
-      <c r="C92" s="15"/>
-      <c r="D92" s="15"/>
+      <c r="C92" s="15">
+        <v>1</v>
+      </c>
+      <c r="D92" s="15">
+        <v>4</v>
+      </c>
       <c r="E92" s="15">
         <v>1</v>
       </c>
@@ -12384,11 +12436,11 @@
         <v>0</v>
       </c>
       <c r="G92" s="15">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H92" s="1">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>7.5</v>
       </c>
       <c r="I92" s="24">
         <v>89</v>
@@ -12398,15 +12450,27 @@
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B93" s="15"/>
-      <c r="C93" s="15"/>
-      <c r="D93" s="15"/>
-      <c r="E93" s="15"/>
-      <c r="F93" s="15"/>
-      <c r="G93" s="15"/>
+      <c r="B93" s="15">
+        <v>2</v>
+      </c>
+      <c r="C93" s="15">
+        <v>0</v>
+      </c>
+      <c r="D93" s="15">
+        <v>2</v>
+      </c>
+      <c r="E93" s="15">
+        <v>1.5</v>
+      </c>
+      <c r="F93" s="15">
+        <v>0</v>
+      </c>
+      <c r="G93" s="15">
+        <v>1.5</v>
+      </c>
       <c r="H93" s="1">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I93" s="24">
         <v>90</v>
@@ -12419,15 +12483,27 @@
       <c r="A94" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B94" s="15"/>
-      <c r="C94" s="15"/>
-      <c r="D94" s="15"/>
-      <c r="E94" s="15"/>
-      <c r="F94" s="15"/>
-      <c r="G94" s="15"/>
+      <c r="B94" s="15">
+        <v>1</v>
+      </c>
+      <c r="C94" s="15">
+        <v>0</v>
+      </c>
+      <c r="D94" s="15">
+        <v>2</v>
+      </c>
+      <c r="E94" s="15">
+        <v>1.5</v>
+      </c>
+      <c r="F94" s="15">
+        <v>0</v>
+      </c>
+      <c r="G94" s="15">
+        <v>0</v>
+      </c>
       <c r="H94" s="1">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="I94" s="24">
         <v>91</v>
@@ -12444,11 +12520,15 @@
       <c r="C95" s="17"/>
       <c r="D95" s="17"/>
       <c r="E95" s="17"/>
-      <c r="F95" s="17"/>
-      <c r="G95" s="17"/>
+      <c r="F95" s="17">
+        <v>0</v>
+      </c>
+      <c r="G95" s="17">
+        <v>3</v>
+      </c>
       <c r="H95" s="1">
         <f t="shared" ref="H95:H101" si="10">SUM(B95:G95)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I95" s="24">
         <v>92</v>
@@ -12460,7 +12540,7 @@
     <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96" s="14">
         <f>SUM(H88:H94)</f>
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="B96" s="17"/>
       <c r="C96" s="17"/>
@@ -12600,7 +12680,7 @@
     <row r="103" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A103" s="19">
         <f>SUM(H95:H101)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B103" s="15"/>
       <c r="C103" s="15"/>

</xml_diff>

<commit_message>
Internal and external strife
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester8.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44FF69A5-6224-4B39-AF38-09287B00E74D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D8D5DA-BBF6-4E28-9C2E-0A346ABD7F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1021,16 +1021,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>157.5</c:v>
+                  <c:v>158</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>324</c:v>
+                  <c:v>330.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>171</c:v>
+                  <c:v>173</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2.5</c:v>
@@ -1544,7 +1544,7 @@
                   <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>3</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="92">
                   <c:v>0</c:v>
@@ -2284,7 +2284,7 @@
                   <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>3</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="92">
                   <c:v>0</c:v>
@@ -3089,7 +3089,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>157.5</c:v>
+                  <c:v>158</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3341,7 +3341,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>324</c:v>
+                  <c:v>330.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3467,7 +3467,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>171</c:v>
+                  <c:v>173</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4313,6 +4313,9 @@
                 <c:pt idx="90">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4654,6 +4657,9 @@
                 <c:pt idx="90">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="91">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4995,6 +5001,9 @@
                 <c:pt idx="90">
                   <c:v>2</c:v>
                 </c:pt>
+                <c:pt idx="91">
+                  <c:v>6.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5335,6 +5344,9 @@
                 </c:pt>
                 <c:pt idx="90">
                   <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9510,8 +9522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE33D67F-891D-4EAD-9F40-3D033E7F434D}">
   <dimension ref="A1:AG122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D95" sqref="D95"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D96" sqref="D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9570,7 +9582,7 @@
       </c>
       <c r="B2" s="5">
         <f>SUM(B4:B166)</f>
-        <v>157.5</v>
+        <v>158</v>
       </c>
       <c r="C2" s="6">
         <f>SUM(C4:C150)</f>
@@ -9578,11 +9590,11 @@
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>324</v>
+        <v>330.5</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="F2" s="9">
         <f>SUM(F4:F150)</f>
@@ -9594,7 +9606,7 @@
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>942.5</v>
+        <v>951.5</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -9678,8 +9690,8 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" s="21">
-        <f>AVERAGE(H4:H94)</f>
-        <v>10.324175824175825</v>
+        <f>AVERAGE(H4:H95)</f>
+        <v>10.342391304347826</v>
       </c>
       <c r="B6" s="15">
         <v>0</v>
@@ -12516,10 +12528,18 @@
       <c r="A95" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B95" s="17"/>
-      <c r="C95" s="17"/>
-      <c r="D95" s="17"/>
-      <c r="E95" s="17"/>
+      <c r="B95" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="C95" s="17">
+        <v>0</v>
+      </c>
+      <c r="D95" s="17">
+        <v>6.5</v>
+      </c>
+      <c r="E95" s="17">
+        <v>2</v>
+      </c>
       <c r="F95" s="17">
         <v>0</v>
       </c>
@@ -12528,7 +12548,7 @@
       </c>
       <c r="H95" s="1">
         <f t="shared" ref="H95:H101" si="10">SUM(B95:G95)</f>
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="I95" s="24">
         <v>92</v>
@@ -12680,7 +12700,7 @@
     <row r="103" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A103" s="19">
         <f>SUM(H95:H101)</f>
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B103" s="15"/>
       <c r="C103" s="15"/>

</xml_diff>

<commit_message>
This is why we should have started early
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester8.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A5648E-3F35-4589-9D68-E9E2B2FF4457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52BFCDE2-A51D-4B3B-A580-A6A90B0CF425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1021,22 +1021,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>163</c:v>
+                  <c:v>163.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>338.5</c:v>
+                  <c:v>347.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>179.5</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>203.5</c:v>
+                  <c:v>204.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1553,7 +1553,7 @@
                   <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>4</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="95">
                   <c:v>0</c:v>
@@ -2293,7 +2293,7 @@
                   <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>4</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="95">
                   <c:v>0</c:v>
@@ -3089,7 +3089,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>163</c:v>
+                  <c:v>163.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3341,7 +3341,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>338.5</c:v>
+                  <c:v>347.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3467,7 +3467,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>179.5</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3719,7 +3719,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>203.5</c:v>
+                  <c:v>204.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4322,6 +4322,9 @@
                 <c:pt idx="93">
                   <c:v>2</c:v>
                 </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5026,7 +5029,7 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>1</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5379,7 +5382,7 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>1</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6083,6 +6086,9 @@
                 </c:pt>
                 <c:pt idx="93">
                   <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9570,8 +9576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE33D67F-891D-4EAD-9F40-3D033E7F434D}">
   <dimension ref="A1:AG122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F99" sqref="F99"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E99" sqref="E99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9630,7 +9636,7 @@
       </c>
       <c r="B2" s="5">
         <f>SUM(B4:B166)</f>
-        <v>163</v>
+        <v>163.5</v>
       </c>
       <c r="C2" s="6">
         <f>SUM(C4:C150)</f>
@@ -9638,11 +9644,11 @@
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>338.5</v>
+        <v>347.5</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
-        <v>179.5</v>
+        <v>180</v>
       </c>
       <c r="F2" s="9">
         <f>SUM(F4:F150)</f>
@@ -9650,11 +9656,11 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(G4:G150)</f>
-        <v>203.5</v>
+        <v>204.5</v>
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>978</v>
+        <v>989</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -12670,23 +12676,27 @@
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B98" s="17"/>
+      <c r="B98" s="17">
+        <v>0.5</v>
+      </c>
       <c r="C98" s="17">
         <v>2</v>
       </c>
       <c r="D98" s="17">
+        <v>10</v>
+      </c>
+      <c r="E98" s="17">
+        <v>1.5</v>
+      </c>
+      <c r="F98" s="17">
+        <v>0</v>
+      </c>
+      <c r="G98" s="17">
         <v>1</v>
       </c>
-      <c r="E98" s="17">
-        <v>1</v>
-      </c>
-      <c r="F98" s="17">
-        <v>0</v>
-      </c>
-      <c r="G98" s="17"/>
       <c r="H98" s="1">
         <f t="shared" si="10"/>
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="I98" s="24">
         <v>95</v>
@@ -12780,7 +12790,7 @@
     <row r="103" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A103" s="19">
         <f>SUM(H95:H101)</f>
-        <v>38.5</v>
+        <v>49.5</v>
       </c>
       <c r="B103" s="15"/>
       <c r="C103" s="15"/>

</xml_diff>